<commit_message>
updated canvascontract to use calculated 14 day and the rack rate in syp section of the contract
</commit_message>
<xml_diff>
--- a/Field Mapping.xlsx
+++ b/Field Mapping.xlsx
@@ -9,14 +9,16 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12435" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="165" uniqueCount="119">
   <si>
     <t>web_strcustr</t>
   </si>
@@ -317,9 +319,6 @@
   </si>
   <si>
     <t>SYP</t>
-  </si>
-  <si>
-    <t>J = junior, '' = standard, S = senior, SYP = student/young professional</t>
   </si>
   <si>
     <t>selectedClub.id / club_id</t>
@@ -351,6 +350,54 @@
   </si>
   <si>
     <t>Each Member on Membership web_proc_InsertAsamembr:</t>
+  </si>
+  <si>
+    <t>J = junior, '' = standard, S = senior, Y = student/young professional</t>
+  </si>
+  <si>
+    <t>Club Name</t>
+  </si>
+  <si>
+    <t>Club ID</t>
+  </si>
+  <si>
+    <t>Database</t>
+  </si>
+  <si>
+    <t>Highpoint</t>
+  </si>
+  <si>
+    <t>NMSW</t>
+  </si>
+  <si>
+    <t>Midtown</t>
+  </si>
+  <si>
+    <t>Downtown</t>
+  </si>
+  <si>
+    <t>Del Norte</t>
+  </si>
+  <si>
+    <t>Riverpoint</t>
+  </si>
+  <si>
+    <t>DTC</t>
+  </si>
+  <si>
+    <t>Denver</t>
+  </si>
+  <si>
+    <t>Tabor Center</t>
+  </si>
+  <si>
+    <t>Flatirons</t>
+  </si>
+  <si>
+    <t>Monaco</t>
+  </si>
+  <si>
+    <t>MAC</t>
   </si>
 </sst>
 </file>
@@ -1048,8 +1095,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1120,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
@@ -1218,7 +1265,7 @@
         <v>70</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.25">
@@ -1241,7 +1288,7 @@
         <v>74</v>
       </c>
       <c r="B30" t="s">
-        <v>97</v>
+        <v>103</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
@@ -1251,7 +1298,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
@@ -1267,7 +1314,7 @@
         <v>82</v>
       </c>
       <c r="B35" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
@@ -1344,7 +1391,7 @@
         <v>54</v>
       </c>
       <c r="B45" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
@@ -1352,7 +1399,7 @@
         <v>92</v>
       </c>
       <c r="B46" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
@@ -1428,4 +1475,143 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="12.42578125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B1" t="s">
+        <v>105</v>
+      </c>
+      <c r="C1" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>107</v>
+      </c>
+      <c r="B2">
+        <v>201</v>
+      </c>
+      <c r="C2" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3">
+        <v>202</v>
+      </c>
+      <c r="C3" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>110</v>
+      </c>
+      <c r="B4">
+        <v>203</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>111</v>
+      </c>
+      <c r="B5">
+        <v>204</v>
+      </c>
+      <c r="C5" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B6">
+        <v>205</v>
+      </c>
+      <c r="C6" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>113</v>
+      </c>
+      <c r="B7">
+        <v>252</v>
+      </c>
+      <c r="C7" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>115</v>
+      </c>
+      <c r="B8">
+        <v>254</v>
+      </c>
+      <c r="C8" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>116</v>
+      </c>
+      <c r="B9">
+        <v>257</v>
+      </c>
+      <c r="C9" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>117</v>
+      </c>
+      <c r="B10">
+        <v>292</v>
+      </c>
+      <c r="C10" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11">
+        <v>375</v>
+      </c>
+      <c r="C11" t="s">
+        <v>118</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>